<commit_message>
Update Diagrama de Gantt Anteproyecto.xlsx
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt Anteproyecto.xlsx
+++ b/Diagrama de Gantt Anteproyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/miguel_amaris_martos_alumnos_upm_es/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/miguel_amaris_martos_alumnos_upm_es/Documents/Áreas/Trabajo y Estudios/2 Grado/PFG/tfg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{354AE251-E014-49F2-B8F1-7E422FF99F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{354AE251-E014-49F2-B8F1-7E422FF99F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09C992B8-0CAE-4276-B1CE-AD8DE07F2B24}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -62,16 +62,16 @@
     <t>Aplicación de JavaCC en prácticas de PIAT</t>
   </si>
   <si>
-    <t>Generación de Documenteación</t>
-  </si>
-  <si>
-    <t>Revisión y mejora de la documentación</t>
-  </si>
-  <si>
     <t>Preparación de la presentación del TFG</t>
   </si>
   <si>
     <t>Evaluación y validación del proyecto</t>
+  </si>
+  <si>
+    <t>Generación de Documentación</t>
+  </si>
+  <si>
+    <t>Revisión y mejora de Documentación</t>
   </si>
 </sst>
 </file>
@@ -449,10 +449,10 @@
                   <c:v>Aplicación de JavaCC en prácticas de PIAT</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Generación de Documenteación</c:v>
+                  <c:v>Generación de Documentación</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Revisión y mejora de la documentación</c:v>
+                  <c:v>Revisión y mejora de Documentación</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Preparación de la presentación del TFG</c:v>
@@ -482,7 +482,7 @@
                   <c:v>45275</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42936</c:v>
+                  <c:v>45274</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>42938</c:v>
@@ -521,10 +521,10 @@
                   <c:v>Aplicación de JavaCC en prácticas de PIAT</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Generación de Documenteación</c:v>
+                  <c:v>Generación de Documentación</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Revisión y mejora de la documentación</c:v>
+                  <c:v>Revisión y mejora de Documentación</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Preparación de la presentación del TFG</c:v>
@@ -554,7 +554,7 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4</c:v>
@@ -636,7 +636,7 @@
         <c:axId val="909698896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45291"/>
+          <c:max val="45342"/>
           <c:min val="45170"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1292,13 +1292,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:colOff>523874</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>471487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
@@ -1628,17 +1628,17 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="2" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -1678,13 +1678,13 @@
         <v>50</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D11" si="0">B3+C3</f>
+        <f t="shared" ref="D3:D7" si="0">B3+C3</f>
         <v>45239</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="12">
         <v>45229</v>
@@ -1697,9 +1697,9 @@
         <v>45259</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="12">
         <v>45275</v>
@@ -1712,24 +1712,24 @@
         <v>45305</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="15">
-        <v>42936</v>
+        <v>45274</v>
       </c>
       <c r="C6" s="16">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D6" s="17">
         <f t="shared" si="0"/>
-        <v>42939</v>
+        <v>45294</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="12">
         <v>42938</v>
@@ -1742,31 +1742,31 @@
         <v>42942</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
       <c r="D8" s="17"/>
     </row>
-    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="1"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
       <c r="D10" s="17"/>
     </row>
-    <row r="11" spans="1:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>4</v>
       </c>
@@ -1775,12 +1775,12 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="22">
-        <v>45291</v>
+        <v>45342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version final de Anteproyecto
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt Anteproyecto.xlsx
+++ b/Diagrama de Gantt Anteproyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/miguel_amaris_martos_alumnos_upm_es/Documents/Áreas/Trabajo y Estudios/2 Grado/PFG/tfg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{354AE251-E014-49F2-B8F1-7E422FF99F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09C992B8-0CAE-4276-B1CE-AD8DE07F2B24}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{354AE251-E014-49F2-B8F1-7E422FF99F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBB54EC2-17CE-4E99-8BE8-9FC7A64E28C9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,10 +482,10 @@
                   <c:v>45275</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45274</c:v>
+                  <c:v>45291</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42938</c:v>
+                  <c:v>45316</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -501,7 +501,9 @@
           <c:order val="1"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -545,19 +547,19 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1628,7 +1630,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1675,11 +1677,11 @@
         <v>45189</v>
       </c>
       <c r="C3" s="1">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D3" s="13">
         <f t="shared" ref="D3:D7" si="0">B3+C3</f>
-        <v>45239</v>
+        <v>45279</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1690,11 +1692,11 @@
         <v>45229</v>
       </c>
       <c r="C4" s="16">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D4" s="17">
         <f t="shared" si="0"/>
-        <v>45259</v>
+        <v>45279</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1717,14 +1719,14 @@
         <v>8</v>
       </c>
       <c r="B6" s="15">
-        <v>45274</v>
+        <v>45291</v>
       </c>
       <c r="C6" s="16">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D6" s="17">
         <f t="shared" si="0"/>
-        <v>45294</v>
+        <v>45316</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1732,14 +1734,14 @@
         <v>9</v>
       </c>
       <c r="B7" s="12">
-        <v>42938</v>
+        <v>45316</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D7" s="13">
         <f t="shared" si="0"/>
-        <v>42942</v>
+        <v>45336</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>